<commit_message>
Estimated FTD amount from September 20 2020 to April 14 2021
</commit_message>
<xml_diff>
--- a/FTD excel.xlsx
+++ b/FTD excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharykolansky/Documents/PythonTools/FTDPharser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD47E1B-BF61-3440-9051-B886EB25FEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FFEBEC-39D0-1449-8631-A6EC32303049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="2380" windowWidth="35840" windowHeight="17440" xr2:uid="{79918374-6A0E-9448-9302-A52C85B8026F}"/>
+    <workbookView xWindow="0" yWindow="2380" windowWidth="35840" windowHeight="17440" xr2:uid="{79918374-6A0E-9448-9302-A52C85B8026F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="output" localSheetId="0">Sheet1!$A$1:$H$283</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="9.9999999999994451E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="63">
   <si>
     <t>SETTLEMENT DATE</t>
   </si>
@@ -242,6 +242,9 @@
   <si>
     <t>8) u/broccaa did work estimating how many FTD were reset with abusive options trading</t>
   </si>
+  <si>
+    <t>9/1/2020 naked short selling occurred</t>
+  </si>
 </sst>
 </file>
 
@@ -276,11 +279,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8725,10 +8729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B41F054-EDA3-C14A-B4CE-0A9415423347}">
-  <dimension ref="A1:V283"/>
+  <dimension ref="A1:W283"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8742,9 +8746,10 @@
     <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -8775,8 +8780,11 @@
       <c r="V1" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W1" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8817,8 +8825,12 @@
         <f>SUM($F$2:$F$283)-$J$41</f>
         <v>77740330</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W2" s="1">
+        <f>SUM($F$2:$F$283)-$J$143</f>
+        <v>47305947</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -8863,8 +8875,12 @@
         <f>47.57*10^6</f>
         <v>47570000</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W3" s="1">
+        <f>47.57*10^6</f>
+        <v>47570000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -8909,8 +8925,12 @@
         <f>V2/V3</f>
         <v>1.6342301870927054</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W4" s="3">
+        <f>W2/W3</f>
+        <v>0.99444916964473407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -8941,7 +8961,7 @@
         <v>275213</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -8972,7 +8992,7 @@
         <v>361452</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -9003,7 +9023,7 @@
         <v>421543</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -9037,7 +9057,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -9071,7 +9091,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -9105,7 +9125,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -9139,7 +9159,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -9173,7 +9193,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -9207,7 +9227,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -9241,7 +9261,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -9275,7 +9295,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>

</xml_diff>